<commit_message>
berekening borstelvermogen verbeterd en diagram toegevoegd
</commit_message>
<xml_diff>
--- a/berekeningen/berekeningen borstelmotorvermogen.xlsx
+++ b/berekeningen/berekeningen borstelmotorvermogen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saxion.sharepoint.com/teams/O365-Course-Team-113290-group5.0/Shared Documents/group 5/berekeningen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svenk\Documents\GitHub\ProjectGearDeburr\berekeningen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{27045640-5866-49D0-8682-24E008A183E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C82C4F3-B447-4F64-88F3-A5866A9F3CFE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EF85C2-065A-4126-A37B-B8FBEA423C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="23385" xr2:uid="{FD37FC2E-9908-4ACD-BFFE-7F2A911E95A5}"/>
   </bookViews>
@@ -35,6 +35,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
@@ -77,9 +99,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>radius borstel</t>
-  </si>
-  <si>
     <t>cm</t>
   </si>
   <si>
@@ -102,6 +121,9 @@
   </si>
   <si>
     <t>Watt</t>
+  </si>
+  <si>
+    <t>r borstel</t>
   </si>
 </sst>
 </file>
@@ -137,8 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -154,6 +179,70 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C009ED-5E6C-4437-ADB2-7E2E436960C3}">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,59 +656,112 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G6">
         <f>C7/100</f>
         <v>0.04</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <f>G5*G6</f>
         <v>1.1772</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
         <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
       </c>
       <c r="G8">
         <f>G7*G4</f>
         <v>369.82828718059045</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B11:C22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>